<commit_message>
Se añaden planos cable datos p10 y p6.67
</commit_message>
<xml_diff>
--- a/P10/Double Side/Escandallo Aveiro P10 DOUBLE SIDE.xlsx
+++ b/P10/Double Side/Escandallo Aveiro P10 DOUBLE SIDE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ingenieria ImasD\Desktop\Proyectos\Cruz-AVEIRO\P10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ingenieria ImasD\Desktop\Proyectos\Cruz-AVEIRO\P10\Double Side\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9E4A79-1BB8-45C9-87D9-14E402BC43F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984B23BA-2668-4F6F-872C-4338C1784EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -877,10 +877,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A6:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A73" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -944,7 +947,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>7</v>
@@ -958,7 +961,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
@@ -1231,12 +1234,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="59" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>